<commit_message>
Misc updates refinery so2 china ind bcoc usa offroad (#297)
* Update to most recent satellite data for SO2 refinery/fugitive emissions. Use refinery throughput for extrapolation
* Update to consistently represent China iron smelting SO2
* Fix swapped China BC/OC Coke emissions
* Add BC/OC controls for recent years in China
* Add usa can rail EF trends (Rename default ship_rail EF input so that more specific shipping EF files have precedence)
* Add USA off-road IEA energy data corrections
* Add MEIC road scaling method
* Added default_iso as an extension method to replace EFs with default EFs from select isos
* Overwrite Ethiopia and Nigeria residential biomass consumption with valued based no UN data instead of IEA.
* Add BC/OC for fossil-fuel fires.
</commit_message>
<xml_diff>
--- a/input/emissions-inventories/China/Fig3_MEIC_detail_Zheng_etal_2018.xlsx
+++ b/input/emissions-inventories/China/Fig3_MEIC_detail_Zheng_etal_2018.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orou913\OneDrive - PNNL\Desktop\CEDS_Repos\CEDS-GBD_MAPS\CEDS\input\emissions-inventories\China\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Documents/Information &amp; Documents/CEDS_Project/CEDS/input/emissions-inventories/China/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397FA779-A736-424D-A78E-CF7F48E62C02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC75051F-F8BA-9349-8CB2-E06BADBE9A61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3468" yWindow="1170" windowWidth="18486" windowHeight="11190" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3460" yWindow="1180" windowWidth="18480" windowHeight="11200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SO2" sheetId="1" r:id="rId1"/>
-    <sheet name="CO2" sheetId="11" r:id="rId2"/>
-    <sheet name="OC" sheetId="10" r:id="rId3"/>
-    <sheet name="BC" sheetId="9" r:id="rId4"/>
-    <sheet name="PM2.5" sheetId="8" r:id="rId5"/>
-    <sheet name="PM10" sheetId="7" r:id="rId6"/>
-    <sheet name="TSP" sheetId="6" r:id="rId7"/>
-    <sheet name="CO" sheetId="5" r:id="rId8"/>
-    <sheet name="NH3" sheetId="4" r:id="rId9"/>
-    <sheet name="NMVOC" sheetId="3" r:id="rId10"/>
-    <sheet name="NOx" sheetId="2" r:id="rId11"/>
+    <sheet name="SO2_org" sheetId="12" r:id="rId2"/>
+    <sheet name="CO2" sheetId="11" r:id="rId3"/>
+    <sheet name="OC" sheetId="10" r:id="rId4"/>
+    <sheet name="BC" sheetId="9" r:id="rId5"/>
+    <sheet name="PM2.5" sheetId="8" r:id="rId6"/>
+    <sheet name="PM10" sheetId="7" r:id="rId7"/>
+    <sheet name="TSP" sheetId="6" r:id="rId8"/>
+    <sheet name="CO" sheetId="5" r:id="rId9"/>
+    <sheet name="NH3" sheetId="4" r:id="rId10"/>
+    <sheet name="NMVOC" sheetId="3" r:id="rId11"/>
+    <sheet name="NOx" sheetId="2" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="21">
   <si>
     <r>
       <t>a. SO</t>
@@ -176,6 +180,12 @@
   </si>
   <si>
     <t>China’s anthropogenic emissions by sector and year</t>
+  </si>
+  <si>
+    <t>ferrous metal SO2</t>
+  </si>
+  <si>
+    <t>(extrapolated from previuos MEIC)</t>
   </si>
 </sst>
 </file>
@@ -333,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -373,6 +383,9 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,29 +669,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.68359375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="12.68359375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83984375" style="1"/>
+    <col min="3" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -701,7 +714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="8">
         <v>2010</v>
@@ -710,7 +723,8 @@
         <v>7.7789700000000002</v>
       </c>
       <c r="D5" s="9">
-        <v>16.400099999999998</v>
+        <f>SO2_org!D5-SO2_org!K5</f>
+        <v>15.494695020080565</v>
       </c>
       <c r="E5" s="9">
         <v>3.3980800000000002</v>
@@ -725,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="8">
         <v>2011</v>
       </c>
@@ -733,7 +747,8 @@
         <v>7.9200600000000003</v>
       </c>
       <c r="D6" s="9">
-        <v>17.331099999999999</v>
+        <f>SO2_org!D6-SO2_org!K6</f>
+        <v>16.501969339732653</v>
       </c>
       <c r="E6" s="9">
         <v>3.5764800000000001</v>
@@ -748,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
         <v>2012</v>
       </c>
@@ -756,7 +771,8 @@
         <v>6.8528099999999998</v>
       </c>
       <c r="D7" s="9">
-        <v>17.608699999999999</v>
+        <f>SO2_org!D7-SO2_org!K7</f>
+        <v>16.905705787292479</v>
       </c>
       <c r="E7" s="9">
         <v>3.7275299999999998</v>
@@ -771,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="8">
         <v>2013</v>
       </c>
@@ -779,7 +795,8 @@
         <v>5.9531700000000001</v>
       </c>
       <c r="D8" s="9">
-        <v>15.837300000000001</v>
+        <f>SO2_org!D8-SO2_org!K8</f>
+        <v>15.090876799730211</v>
       </c>
       <c r="E8" s="9">
         <v>3.3547099999999999</v>
@@ -794,7 +811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="8">
         <v>2014</v>
       </c>
@@ -802,7 +819,8 @@
         <v>4.9068199999999997</v>
       </c>
       <c r="D9" s="9">
-        <v>12.133599999999999</v>
+        <f>SO2_org!D9-SO2_org!K9</f>
+        <v>11.384817406705894</v>
       </c>
       <c r="E9" s="9">
         <v>3.1051500000000001</v>
@@ -817,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="8">
         <v>2015</v>
       </c>
@@ -825,7 +843,8 @@
         <v>3.9346100000000002</v>
       </c>
       <c r="D10" s="9">
-        <v>9.8079400000000003</v>
+        <f>SO2_org!D10-SO2_org!K10</f>
+        <v>9.0825887287148159</v>
       </c>
       <c r="E10" s="9">
         <v>2.86287</v>
@@ -840,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="8">
         <v>2016</v>
       </c>
@@ -848,7 +867,8 @@
         <v>2.6688399999999999</v>
       </c>
       <c r="D11" s="9">
-        <v>7.6727600000000002</v>
+        <f>SO2_org!D11-SO2_org!K11</f>
+        <v>6.9360156614653476</v>
       </c>
       <c r="E11" s="9">
         <v>2.7117399999999998</v>
@@ -863,7 +883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" s="11">
         <v>2017</v>
       </c>
@@ -871,7 +891,8 @@
         <v>1.83047</v>
       </c>
       <c r="D12" s="12">
-        <v>5.9697699999999996</v>
+        <f>SO2_org!D12-SO2_org!K12</f>
+        <v>5.2211227387201831</v>
       </c>
       <c r="E12" s="12">
         <v>2.3702800000000002</v>
@@ -886,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
     </row>
   </sheetData>
@@ -896,23 +917,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C25AF01-0B3C-D647-9C6A-799D8FE75E61}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287EAD4B-F67B-C04F-BCE5-00AC0B8BF9C9}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -921,7 +940,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -944,188 +963,188 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>2010</v>
       </c>
       <c r="B5" s="9">
-        <v>6.6839999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="C5" s="9">
-        <v>7.8731999999999998</v>
+        <v>0.27356999999999998</v>
       </c>
       <c r="D5" s="9">
-        <v>4.9947600000000003</v>
+        <v>0.42655999999999999</v>
       </c>
       <c r="E5" s="9">
-        <v>6.0595600000000003</v>
+        <v>2.6679999999999999E-2</v>
       </c>
       <c r="F5" s="9">
-        <v>6.8702300000000003</v>
+        <v>0</v>
       </c>
       <c r="G5" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>9.4552800000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>2011</v>
       </c>
       <c r="B6" s="9">
-        <v>7.775E-2</v>
+        <v>0</v>
       </c>
       <c r="C6" s="9">
-        <v>8.4582200000000007</v>
+        <v>0.29355999999999999</v>
       </c>
       <c r="D6" s="9">
-        <v>5.0064299999999999</v>
+        <v>0.42096</v>
       </c>
       <c r="E6" s="9">
-        <v>5.75101</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="F6" s="9">
-        <v>7.6244500000000004</v>
+        <v>0</v>
       </c>
       <c r="G6" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>9.8011900000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>2012</v>
       </c>
       <c r="B7" s="9">
-        <v>7.7660000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="C7" s="9">
-        <v>8.8575800000000005</v>
+        <v>0.33835999999999999</v>
       </c>
       <c r="D7" s="9">
-        <v>5.0143399999999998</v>
+        <v>0.41675000000000001</v>
       </c>
       <c r="E7" s="9">
-        <v>5.6277900000000001</v>
+        <v>3.134E-2</v>
       </c>
       <c r="F7" s="9">
-        <v>8.5126500000000007</v>
+        <v>0</v>
       </c>
       <c r="G7" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>9.9147999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>2013</v>
       </c>
       <c r="B8" s="9">
-        <v>7.9219999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="C8" s="9">
-        <v>9.0784500000000001</v>
+        <v>0.35313</v>
       </c>
       <c r="D8" s="9">
-        <v>4.7831400000000004</v>
+        <v>0.39949000000000001</v>
       </c>
       <c r="E8" s="9">
-        <v>5.5841200000000004</v>
+        <v>3.5029999999999999E-2</v>
       </c>
       <c r="F8" s="9">
-        <v>8.5682100000000005</v>
+        <v>0</v>
       </c>
       <c r="G8" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>9.8470399999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>2014</v>
       </c>
       <c r="B9" s="9">
-        <v>7.757E-2</v>
+        <v>0</v>
       </c>
       <c r="C9" s="9">
-        <v>9.2009000000000007</v>
+        <v>0.33751999999999999</v>
       </c>
       <c r="D9" s="9">
-        <v>4.5453700000000001</v>
+        <v>0.37905</v>
       </c>
       <c r="E9" s="9">
-        <v>5.1157599999999999</v>
+        <v>3.6119999999999999E-2</v>
       </c>
       <c r="F9" s="9">
-        <v>10.128399999999999</v>
+        <v>0</v>
       </c>
       <c r="G9" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>9.7972000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>2015</v>
       </c>
       <c r="B10" s="9">
-        <v>7.7439999999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="C10" s="9">
-        <v>9.3617799999999995</v>
+        <v>0.36177999999999999</v>
       </c>
       <c r="D10" s="9">
-        <v>4.2194700000000003</v>
+        <v>0.35420000000000001</v>
       </c>
       <c r="E10" s="9">
-        <v>5.38748</v>
+        <v>4.122E-2</v>
       </c>
       <c r="F10" s="9">
-        <v>9.4519599999999997</v>
+        <v>0</v>
       </c>
       <c r="G10" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>9.7291299999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>2016</v>
       </c>
       <c r="B11" s="9">
-        <v>7.9570000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="C11" s="9">
-        <v>9.3094400000000004</v>
+        <v>0.31664999999999999</v>
       </c>
       <c r="D11" s="9">
-        <v>3.8974299999999999</v>
+        <v>0.33023999999999998</v>
       </c>
       <c r="E11" s="9">
-        <v>4.9610799999999999</v>
+        <v>4.2209999999999998E-2</v>
       </c>
       <c r="F11" s="9">
-        <v>10.1088</v>
+        <v>0</v>
       </c>
       <c r="G11" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>9.6379199999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2017</v>
       </c>
       <c r="B12" s="12">
-        <v>8.473E-2</v>
+        <v>0</v>
       </c>
       <c r="C12" s="12">
-        <v>9.7076200000000004</v>
+        <v>0.30481999999999998</v>
       </c>
       <c r="D12" s="12">
-        <v>3.60338</v>
+        <v>0.30904999999999999</v>
       </c>
       <c r="E12" s="12">
-        <v>4.7861000000000002</v>
+        <v>4.3639999999999998E-2</v>
       </c>
       <c r="F12" s="12">
-        <v>10.4353</v>
+        <v>0</v>
       </c>
       <c r="G12" s="13">
-        <v>0</v>
+        <v>9.6115600000000008</v>
       </c>
     </row>
   </sheetData>
@@ -1134,6 +1153,244 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C25AF01-0B3C-D647-9C6A-799D8FE75E61}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>2010</v>
+      </c>
+      <c r="B5" s="9">
+        <v>6.6839999999999997E-2</v>
+      </c>
+      <c r="C5" s="9">
+        <v>7.8731999999999998</v>
+      </c>
+      <c r="D5" s="9">
+        <v>4.9947600000000003</v>
+      </c>
+      <c r="E5" s="9">
+        <v>6.0595600000000003</v>
+      </c>
+      <c r="F5" s="9">
+        <v>6.8702300000000003</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>2011</v>
+      </c>
+      <c r="B6" s="9">
+        <v>7.775E-2</v>
+      </c>
+      <c r="C6" s="9">
+        <v>8.4582200000000007</v>
+      </c>
+      <c r="D6" s="9">
+        <v>5.0064299999999999</v>
+      </c>
+      <c r="E6" s="9">
+        <v>5.75101</v>
+      </c>
+      <c r="F6" s="9">
+        <v>7.6244500000000004</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>2012</v>
+      </c>
+      <c r="B7" s="9">
+        <v>7.7660000000000007E-2</v>
+      </c>
+      <c r="C7" s="9">
+        <v>8.8575800000000005</v>
+      </c>
+      <c r="D7" s="9">
+        <v>5.0143399999999998</v>
+      </c>
+      <c r="E7" s="9">
+        <v>5.6277900000000001</v>
+      </c>
+      <c r="F7" s="9">
+        <v>8.5126500000000007</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>2013</v>
+      </c>
+      <c r="B8" s="9">
+        <v>7.9219999999999999E-2</v>
+      </c>
+      <c r="C8" s="9">
+        <v>9.0784500000000001</v>
+      </c>
+      <c r="D8" s="9">
+        <v>4.7831400000000004</v>
+      </c>
+      <c r="E8" s="9">
+        <v>5.5841200000000004</v>
+      </c>
+      <c r="F8" s="9">
+        <v>8.5682100000000005</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>2014</v>
+      </c>
+      <c r="B9" s="9">
+        <v>7.757E-2</v>
+      </c>
+      <c r="C9" s="9">
+        <v>9.2009000000000007</v>
+      </c>
+      <c r="D9" s="9">
+        <v>4.5453700000000001</v>
+      </c>
+      <c r="E9" s="9">
+        <v>5.1157599999999999</v>
+      </c>
+      <c r="F9" s="9">
+        <v>10.128399999999999</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>2015</v>
+      </c>
+      <c r="B10" s="9">
+        <v>7.7439999999999995E-2</v>
+      </c>
+      <c r="C10" s="9">
+        <v>9.3617799999999995</v>
+      </c>
+      <c r="D10" s="9">
+        <v>4.2194700000000003</v>
+      </c>
+      <c r="E10" s="9">
+        <v>5.38748</v>
+      </c>
+      <c r="F10" s="9">
+        <v>9.4519599999999997</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>2016</v>
+      </c>
+      <c r="B11" s="9">
+        <v>7.9570000000000002E-2</v>
+      </c>
+      <c r="C11" s="9">
+        <v>9.3094400000000004</v>
+      </c>
+      <c r="D11" s="9">
+        <v>3.8974299999999999</v>
+      </c>
+      <c r="E11" s="9">
+        <v>4.9610799999999999</v>
+      </c>
+      <c r="F11" s="9">
+        <v>10.1088</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>2017</v>
+      </c>
+      <c r="B12" s="12">
+        <v>8.473E-2</v>
+      </c>
+      <c r="C12" s="12">
+        <v>9.7076200000000004</v>
+      </c>
+      <c r="D12" s="12">
+        <v>3.60338</v>
+      </c>
+      <c r="E12" s="12">
+        <v>4.7861000000000002</v>
+      </c>
+      <c r="F12" s="12">
+        <v>10.4353</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6974A5B-257A-564E-AA58-EDDBF185CB2A}">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -1141,14 +1398,14 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1159,7 +1416,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1182,7 +1439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>2010</v>
       </c>
@@ -1205,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>2011</v>
       </c>
@@ -1228,7 +1485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>2012</v>
       </c>
@@ -1251,7 +1508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>2013</v>
       </c>
@@ -1274,7 +1531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>2014</v>
       </c>
@@ -1297,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>2015</v>
       </c>
@@ -1320,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>2016</v>
       </c>
@@ -1343,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2017</v>
       </c>
@@ -1372,19 +1629,297 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CDA42F-4975-D240-8030-F45909FC5356}">
+  <dimension ref="A2:L65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8">
+        <v>2010</v>
+      </c>
+      <c r="C5" s="9">
+        <v>7.7789700000000002</v>
+      </c>
+      <c r="D5" s="9">
+        <v>16.400099999999998</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3.3980800000000002</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0.23431299999999999</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.90540497991943358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B6" s="8">
+        <v>2011</v>
+      </c>
+      <c r="C6" s="9">
+        <v>7.9200600000000003</v>
+      </c>
+      <c r="D6" s="9">
+        <v>17.331099999999999</v>
+      </c>
+      <c r="E6" s="9">
+        <v>3.5764800000000001</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.25197999999999998</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.82913066026734716</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="8">
+        <v>2012</v>
+      </c>
+      <c r="C7" s="9">
+        <v>6.8528099999999998</v>
+      </c>
+      <c r="D7" s="9">
+        <v>17.608699999999999</v>
+      </c>
+      <c r="E7" s="9">
+        <v>3.7275299999999998</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0.27370100000000003</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.70299421270751949</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="8">
+        <v>2013</v>
+      </c>
+      <c r="C8" s="9">
+        <v>5.9531700000000001</v>
+      </c>
+      <c r="D8" s="9">
+        <v>15.837300000000001</v>
+      </c>
+      <c r="E8" s="9">
+        <v>3.3547099999999999</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.29019099999999998</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.74642320026979103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="8">
+        <v>2014</v>
+      </c>
+      <c r="C9" s="9">
+        <v>4.9068199999999997</v>
+      </c>
+      <c r="D9" s="9">
+        <v>12.133599999999999</v>
+      </c>
+      <c r="E9" s="9">
+        <v>3.1051500000000001</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.29636899999999999</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.74878259329410557</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="8">
+        <v>2015</v>
+      </c>
+      <c r="C10" s="9">
+        <v>3.9346100000000002</v>
+      </c>
+      <c r="D10" s="9">
+        <v>9.8079400000000003</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2.86287</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.315863</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.72535127128518384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="8">
+        <v>2016</v>
+      </c>
+      <c r="C11" s="9">
+        <v>2.6688399999999999</v>
+      </c>
+      <c r="D11" s="9">
+        <v>7.6727600000000002</v>
+      </c>
+      <c r="E11" s="9">
+        <v>2.7117399999999998</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.320577</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.73674433853465293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B12" s="11">
+        <v>2017</v>
+      </c>
+      <c r="C12" s="12">
+        <v>1.83047</v>
+      </c>
+      <c r="D12" s="12">
+        <v>5.9697699999999996</v>
+      </c>
+      <c r="E12" s="12">
+        <v>2.3702800000000002</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0.33292500000000003</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="13">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.74864726127981651</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K13" s="1">
+        <v>0.80890148020000541</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63D27BB-F11D-E647-9621-A1ECD69FD3E8}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1395,7 +1930,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1418,7 +1953,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>2010</v>
       </c>
@@ -1441,7 +1976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>2011</v>
       </c>
@@ -1464,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>2012</v>
       </c>
@@ -1487,7 +2022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>2013</v>
       </c>
@@ -1510,7 +2045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>2014</v>
       </c>
@@ -1533,7 +2068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>2015</v>
       </c>
@@ -1556,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>2016</v>
       </c>
@@ -1579,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2017</v>
       </c>
@@ -1607,20 +2142,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61DB452-9226-124E-BF75-17D92A33F96A}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1631,7 +2166,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1654,7 +2189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>2010</v>
       </c>
@@ -1677,7 +2212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>2011</v>
       </c>
@@ -1700,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>2012</v>
       </c>
@@ -1723,7 +2258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>2013</v>
       </c>
@@ -1746,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>2014</v>
       </c>
@@ -1769,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>2015</v>
       </c>
@@ -1792,7 +2327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>2016</v>
       </c>
@@ -1815,7 +2350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2017</v>
       </c>
@@ -1843,20 +2378,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422717CF-610C-BD40-876B-942F730329B7}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1867,7 +2402,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1890,7 +2425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>2010</v>
       </c>
@@ -1913,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>2011</v>
       </c>
@@ -1936,7 +2471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>2012</v>
       </c>
@@ -1959,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>2013</v>
       </c>
@@ -1982,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>2014</v>
       </c>
@@ -2005,7 +2540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>2015</v>
       </c>
@@ -2028,7 +2563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>2016</v>
       </c>
@@ -2051,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2017</v>
       </c>
@@ -2079,20 +2614,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C408C61-6A84-1343-8CDD-E0857524E203}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -2103,7 +2638,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -2126,7 +2661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>2010</v>
       </c>
@@ -2149,7 +2684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>2011</v>
       </c>
@@ -2172,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>2012</v>
       </c>
@@ -2195,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>2013</v>
       </c>
@@ -2218,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>2014</v>
       </c>
@@ -2241,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>2015</v>
       </c>
@@ -2264,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>2016</v>
       </c>
@@ -2287,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2017</v>
       </c>
@@ -2315,20 +2850,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129B1789-4AA1-D24C-A58F-D17EA2F13B2B}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -2339,7 +2874,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -2362,7 +2897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>2010</v>
       </c>
@@ -2385,7 +2920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>2011</v>
       </c>
@@ -2408,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>2012</v>
       </c>
@@ -2431,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>2013</v>
       </c>
@@ -2454,7 +2989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>2014</v>
       </c>
@@ -2477,7 +3012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>2015</v>
       </c>
@@ -2500,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>2016</v>
       </c>
@@ -2523,7 +3058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2017</v>
       </c>
@@ -2551,7 +3086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD1028B-3649-774F-87E3-71429F623368}">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -2559,14 +3094,14 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -2577,7 +3112,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -2600,7 +3135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>2010</v>
       </c>
@@ -2623,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>2011</v>
       </c>
@@ -2646,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>2012</v>
       </c>
@@ -2669,7 +3204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>2013</v>
       </c>
@@ -2692,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>2014</v>
       </c>
@@ -2715,7 +3250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>2015</v>
       </c>
@@ -2738,7 +3273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>2016</v>
       </c>
@@ -2761,7 +3296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2017</v>
       </c>
@@ -2789,20 +3324,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10801123-3CA9-D144-8BF4-53EE2596168D}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -2813,7 +3348,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -2836,7 +3371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>2010</v>
       </c>
@@ -2859,7 +3394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>2011</v>
       </c>
@@ -2882,7 +3417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>2012</v>
       </c>
@@ -2905,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>2013</v>
       </c>
@@ -2928,7 +3463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>2014</v>
       </c>
@@ -2951,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>2015</v>
       </c>
@@ -2974,7 +3509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>2016</v>
       </c>
@@ -2997,7 +3532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2017</v>
       </c>
@@ -3018,242 +3553,6 @@
       </c>
       <c r="G12" s="13">
         <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287EAD4B-F67B-C04F-BCE5-00AC0B8BF9C9}">
-  <dimension ref="A1:G12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8">
-        <v>2010</v>
-      </c>
-      <c r="B5" s="9">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0.27356999999999998</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0.42655999999999999</v>
-      </c>
-      <c r="E5" s="9">
-        <v>2.6679999999999999E-2</v>
-      </c>
-      <c r="F5" s="9">
-        <v>0</v>
-      </c>
-      <c r="G5" s="10">
-        <v>9.4552800000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="8">
-        <v>2011</v>
-      </c>
-      <c r="B6" s="9">
-        <v>0</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0.29355999999999999</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0.42096</v>
-      </c>
-      <c r="E6" s="9">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0</v>
-      </c>
-      <c r="G6" s="10">
-        <v>9.8011900000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="8">
-        <v>2012</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0.33835999999999999</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0.41675000000000001</v>
-      </c>
-      <c r="E7" s="9">
-        <v>3.134E-2</v>
-      </c>
-      <c r="F7" s="9">
-        <v>0</v>
-      </c>
-      <c r="G7" s="10">
-        <v>9.9147999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="8">
-        <v>2013</v>
-      </c>
-      <c r="B8" s="9">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0.35313</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0.39949000000000001</v>
-      </c>
-      <c r="E8" s="9">
-        <v>3.5029999999999999E-2</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0</v>
-      </c>
-      <c r="G8" s="10">
-        <v>9.8470399999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="8">
-        <v>2014</v>
-      </c>
-      <c r="B9" s="9">
-        <v>0</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0.33751999999999999</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0.37905</v>
-      </c>
-      <c r="E9" s="9">
-        <v>3.6119999999999999E-2</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="10">
-        <v>9.7972000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="8">
-        <v>2015</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0.36177999999999999</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0.35420000000000001</v>
-      </c>
-      <c r="E10" s="9">
-        <v>4.122E-2</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0</v>
-      </c>
-      <c r="G10" s="10">
-        <v>9.7291299999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="8">
-        <v>2016</v>
-      </c>
-      <c r="B11" s="9">
-        <v>0</v>
-      </c>
-      <c r="C11" s="9">
-        <v>0.31664999999999999</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0.33023999999999998</v>
-      </c>
-      <c r="E11" s="9">
-        <v>4.2209999999999998E-2</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
-      <c r="G11" s="10">
-        <v>9.6379199999999994</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="11">
-        <v>2017</v>
-      </c>
-      <c r="B12" s="12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="12">
-        <v>0.30481999999999998</v>
-      </c>
-      <c r="D12" s="12">
-        <v>0.30904999999999999</v>
-      </c>
-      <c r="E12" s="12">
-        <v>4.3639999999999998E-2</v>
-      </c>
-      <c r="F12" s="12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="13">
-        <v>9.6115600000000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>